<commit_message>
update RDA with lidar data
</commit_message>
<xml_diff>
--- a/Carbon_Calculations/IPCC_Carbon_Calculations.xlsx
+++ b/Carbon_Calculations/IPCC_Carbon_Calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/cmptrsn2_illinois_edu/Documents/Chapter2/Floodplain-Experiment-Repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/cmptrsn2_illinois_edu/Documents/Chapter2/Floodplain-Experiment-Repo/Carbon_Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1363" documentId="8_{81C5A17B-0AA7-4E1F-9EEB-1F73114DAE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3437609C-A3E7-4147-A064-41836BB593D1}"/>
+  <xr:revisionPtr revIDLastSave="1380" documentId="8_{81C5A17B-0AA7-4E1F-9EEB-1F73114DAE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C315032-43CE-4C2C-A334-F72D67020DD8}"/>
   <bookViews>
-    <workbookView xWindow="42060" yWindow="-3015" windowWidth="15540" windowHeight="15750" xr2:uid="{2C906CBC-631A-4B26-833B-3AA2F3C7757D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{2C906CBC-631A-4B26-833B-3AA2F3C7757D}"/>
   </bookViews>
   <sheets>
     <sheet name="Joslin estimates" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="91">
   <si>
     <t>Natural wetlands</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>Table 3.2.4/3.3.3 (IPCC Good Practice Guidance for LULUCF) / Table 2.3 (2006 IPCC Guidelines for National Greenhouse Gas Inventories)</t>
+  </si>
+  <si>
+    <t>Total live woody carbon</t>
   </si>
 </sst>
 </file>
@@ -335,12 +338,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -355,16 +364,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,10 +387,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -703,711 +706,746 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECBA9F9-5B1E-4DE3-BE7E-98B24B386112}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="59" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="6" customWidth="1"/>
-    <col min="5" max="6" width="15.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="48.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.88671875" style="6"/>
-    <col min="12" max="12" width="10" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="59" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1">
         <v>1998</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2">
         <v>2023</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2">
         <v>0.69</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2">
         <f>D2-G2</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2">
         <f>D2+G2</f>
         <v>0.80999999999999994</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2">
         <v>0.12</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3">
         <f>B2-B1</f>
         <v>25</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3">
         <v>0.92</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3">
         <f>D3-G3</f>
         <v>0.78</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3">
         <f>D3+G3</f>
         <v>1.06</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="6" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5">
         <v>0.82</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5">
         <f>D5-G5</f>
         <v>0.64999999999999991</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5">
         <f>D5+G5</f>
         <v>0.99</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5">
         <v>0.17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7">
         <f>C26/$D$10</f>
         <v>0.26</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7">
         <f>D26/$D$10</f>
         <v>0.04</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7">
         <f>E26/$D$10</f>
         <v>0.62</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8">
         <v>34.700000000000003</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="6" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9">
         <v>0.47799999999999998</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9">
         <v>0.434</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9">
         <v>0.52</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10">
         <v>50</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="3">
         <f>C28/$D$10</f>
         <v>0.33173200000000003</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="3">
         <f>D28/$D$10</f>
         <v>0.30119600000000002</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="3">
         <f>E28/$D$10</f>
         <v>0.36088000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="6" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12">
         <v>4</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12">
         <v>0.5</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12">
         <v>8</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C13" s="6" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13">
         <v>4</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13">
         <v>0.5</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13">
         <v>7.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C14" s="6" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14">
         <v>0.48</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14">
         <v>0.46</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14">
         <v>0.5</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="6" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15">
         <v>130</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15">
         <v>50</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15">
         <v>200</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C16" s="6" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16">
         <v>60</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16">
         <v>10</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16">
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C17" s="6" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17">
         <v>0.46</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17">
         <v>0.12</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17">
         <v>0.93</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C18" s="6" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18">
         <v>0.23</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18">
         <v>0.13</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18">
         <v>0.37</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C19" s="6" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19">
         <v>0.24</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19">
         <v>0.17</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19">
         <v>0.44</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="6">
         <f>C24*D2*D3*D4</f>
         <v>55.862400000000001</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="6">
         <f>D24*E2*E3*E4</f>
         <v>39.1248</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="6">
         <f>E24*F2*F3*F4</f>
         <v>75.55680000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="6">
         <f>C24*D5</f>
         <v>72.16</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <f>D24*E5</f>
         <v>57.199999999999989</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <f>E24*F5</f>
         <v>87.12</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
+    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="6">
         <v>88</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="6">
         <v>88</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="6">
         <v>88</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="6">
         <f>D7*$B$3</f>
         <v>6.5</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="6">
         <f>E7*$B$3</f>
         <v>1</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="6">
         <f>F7*$B$3</f>
         <v>15.5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
+    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="6">
         <v>13</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="6">
         <v>2</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="6">
         <v>31</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="6">
         <f>D11*$B$3</f>
         <v>8.2933000000000003</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="6">
         <f t="shared" ref="D27:E27" si="0">E11*$B$3</f>
         <v>7.5299000000000005</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="6">
         <f t="shared" si="0"/>
         <v>9.0220000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="6" t="s">
+    <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="6">
         <f>$D$8*D9</f>
         <v>16.586600000000001</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="6">
         <f>$D$8*E9</f>
         <v>15.059800000000001</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="6">
         <f>$D$8*F9</f>
         <v>18.044</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>87</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="2">
         <f>C25+C27</f>
         <v>14.7933</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="2">
         <f t="shared" ref="D29:E29" si="1">D25+D27</f>
         <v>8.5299000000000014</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="2">
         <f t="shared" si="1"/>
         <v>24.521999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="6" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="2">
         <f>C26+C28</f>
         <v>29.586600000000001</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="2">
         <f t="shared" ref="D30:E30" si="2">D26+D28</f>
         <v>17.059800000000003</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="2">
         <f t="shared" si="2"/>
         <v>49.043999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="2">
         <f>D12*20+D13*5</f>
         <v>100</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="2">
         <f t="shared" ref="D31:E31" si="3">E12*20+E13*5</f>
         <v>12.5</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="2">
         <f t="shared" si="3"/>
         <v>197.5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="6" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32">
         <f>D15</f>
         <v>130</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32">
         <f>E15</f>
         <v>50</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32">
         <f>F15</f>
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="6">
         <f>C31*D14</f>
         <v>48</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="6">
         <f>D31*E14</f>
         <v>5.75</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="6">
         <f>E31*F14</f>
         <v>98.75</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="6" t="s">
+    <row r="34" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="6">
         <f>C32*D14</f>
         <v>62.4</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="6">
         <f>D32*E14</f>
         <v>23</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="6">
         <f>E32*F14</f>
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="3">
         <f>IF(C31&lt;75, $D$17, IF(C31&gt;150, $D$19, $D$18))</f>
         <v>0.23</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="3">
         <f>IF(D31&lt;75, $E$17, IF(D31&gt;150, $E$19, $E$18))</f>
         <v>0.12</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="3">
         <f>IF(E31&lt;75, $F$17, IF(E31&gt;150, $F$19, $F$18))</f>
         <v>0.44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="6" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="3">
         <f>IF(C32&lt;75, $D$17, IF(C32&gt;150, $D$19, $D$18))</f>
         <v>0.23</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="3">
         <f>IF(D32&lt;75, $E$17, IF(D32&gt;150, $E$19, $E$18))</f>
         <v>0.12</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="3">
         <f>IF(E32&lt;75, $F$17, IF(E32&gt;150, $F$19, $F$18))</f>
         <v>0.44</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
+    <row r="37" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="6">
         <f t="shared" ref="C37:E38" si="4">C33*C35</f>
         <v>11.040000000000001</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="6">
         <f t="shared" si="4"/>
         <v>0.69</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="6">
         <f t="shared" si="4"/>
         <v>43.45</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="6" t="s">
+    <row r="38" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="6">
         <f t="shared" si="4"/>
         <v>14.352</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="6">
         <f t="shared" si="4"/>
         <v>2.76</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="6">
         <f t="shared" si="4"/>
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="2">
+        <f>C33+C37</f>
+        <v>59.04</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" ref="D39:E39" si="5">D33+D37</f>
+        <v>6.4399999999999995</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="5"/>
+        <v>142.19999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="2">
+        <f>C34+C38</f>
+        <v>76.751999999999995</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" ref="D40:E40" si="6">D34+D38</f>
+        <v>25.759999999999998</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="6"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="8">
-        <f t="shared" ref="C39:E40" si="5">C23+C25+C27+C33+C37</f>
+      <c r="C41" s="6">
+        <f t="shared" ref="C41:E42" si="7">C23+C25+C27+C33+C37</f>
         <v>145.9933</v>
       </c>
-      <c r="D39" s="8">
-        <f t="shared" si="5"/>
+      <c r="D41" s="6">
+        <f t="shared" si="7"/>
         <v>72.169899999999984</v>
       </c>
-      <c r="E39" s="8">
-        <f t="shared" si="5"/>
+      <c r="E41" s="6">
+        <f t="shared" si="7"/>
         <v>253.84199999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="6" t="s">
+    <row r="42" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="8">
-        <f t="shared" si="5"/>
+      <c r="C42" s="6">
+        <f t="shared" si="7"/>
         <v>194.33860000000001</v>
       </c>
-      <c r="D40" s="8">
-        <f>D24+D26+D28+D34+D38</f>
+      <c r="D42" s="6">
+        <f t="shared" si="7"/>
         <v>130.81979999999999</v>
       </c>
-      <c r="E40" s="8">
-        <f t="shared" si="5"/>
+      <c r="E42" s="6">
+        <f t="shared" si="7"/>
         <v>281.04399999999998</v>
       </c>
     </row>
@@ -1424,12 +1462,12 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>78</v>
       </c>
@@ -1437,7 +1475,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1472,7 +1510,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1493,7 +1531,7 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1530,7 +1568,7 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1567,7 +1605,7 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1604,7 +1642,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1641,7 +1679,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1662,7 +1700,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
@@ -1683,7 +1721,7 @@
         <v>531.4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>81</v>
       </c>
@@ -1696,7 +1734,7 @@
         <v>5639.5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>82</v>
       </c>
@@ -1705,7 +1743,7 @@
         <v>0.47792372881355932</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
@@ -1714,7 +1752,7 @@
         <v>0.434</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -1736,17 +1774,17 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1772,7 +1810,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1800,7 +1838,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -1826,7 +1864,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1847,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>35</v>
       </c>
@@ -1866,12 +1904,12 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>45</v>
       </c>
@@ -1891,7 +1929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>38</v>
       </c>
@@ -1902,7 +1940,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>50</v>
       </c>
@@ -1910,7 +1948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>51</v>
       </c>
@@ -1919,7 +1957,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>48</v>
       </c>
@@ -1936,7 +1974,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>47</v>
       </c>
@@ -1947,7 +1985,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>52</v>
       </c>
@@ -1964,7 +2002,7 @@
         <v>0.35602200000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>39</v>
       </c>
@@ -1981,7 +2019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>40</v>
       </c>
@@ -1998,7 +2036,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>25</v>
       </c>
@@ -2012,7 +2050,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>41</v>
       </c>
@@ -2029,7 +2067,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>55</v>
       </c>
@@ -2043,7 +2081,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -2063,7 +2101,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2083,7 +2121,7 @@
         <v>75.55680000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>36</v>
       </c>
@@ -2100,7 +2138,7 @@
         <v>87.12</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -2117,7 +2155,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2137,7 +2175,7 @@
         <v>10.23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>18</v>
       </c>
@@ -2154,7 +2192,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -2174,7 +2212,7 @@
         <v>5.8743630000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>21</v>
       </c>
@@ -2191,7 +2229,7 @@
         <v>17.801100000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2211,7 +2249,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>23</v>
       </c>
@@ -2228,7 +2266,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -2248,7 +2286,7 @@
         <v>198.22436300000001</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>34</v>
       </c>
@@ -2265,7 +2303,7 @@
         <v>236.80109999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -2285,7 +2323,7 @@
         <v>145.95236299999999</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
moved files not used in manuscript, made csv columns more consistent
</commit_message>
<xml_diff>
--- a/Carbon_Calculations/IPCC_Carbon_Calculations.xlsx
+++ b/Carbon_Calculations/IPCC_Carbon_Calculations.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/cmptrsn2_illinois_edu/Documents/Chapter2/Floodplain-Experiment-Repo/Carbon_Calculations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/cmptrsn2_illinois_edu/Documents/Chapter2/Floodplain-Experiment-Repo/Tree_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1380" documentId="8_{81C5A17B-0AA7-4E1F-9EEB-1F73114DAE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C315032-43CE-4C2C-A334-F72D67020DD8}"/>
+  <xr:revisionPtr revIDLastSave="1385" documentId="8_{81C5A17B-0AA7-4E1F-9EEB-1F73114DAE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B132E2AB-BAAE-4655-8D4E-2FDF1964FB49}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{2C906CBC-631A-4B26-833B-3AA2F3C7757D}"/>
+    <workbookView xWindow="28680" yWindow="-3420" windowWidth="29040" windowHeight="15990" xr2:uid="{2C906CBC-631A-4B26-833B-3AA2F3C7757D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Joslin estimates" sheetId="1" r:id="rId1"/>
+    <sheet name="Henry County estimates" sheetId="1" r:id="rId1"/>
     <sheet name="Harmon et al. 2023" sheetId="3" r:id="rId2"/>
-    <sheet name="Summer 2024 estimates" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>Natural wetlands</t>
   </si>
@@ -73,9 +72,6 @@
     <t xml:space="preserve">Annual crops </t>
   </si>
   <si>
-    <t>Mean C stock estimate</t>
-  </si>
-  <si>
     <t>Lower bound</t>
   </si>
   <si>
@@ -112,33 +108,12 @@
     <t>Mature temperate forest (&gt;20 y)</t>
   </si>
   <si>
-    <t>Aboveground living biomass</t>
-  </si>
-  <si>
     <t>Live wood C concentration</t>
   </si>
   <si>
-    <t>Table 4.9</t>
-  </si>
-  <si>
-    <t>Table 4.7</t>
-  </si>
-  <si>
-    <t>Table 4.3</t>
-  </si>
-  <si>
-    <t>Table 5.5</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
-    <t>Table 2.2</t>
-  </si>
-  <si>
-    <t>Table 2.3</t>
-  </si>
-  <si>
     <t>Restored</t>
   </si>
   <si>
@@ -184,34 +159,10 @@
     <t>Broadleaf deciduous forest transition period (y)</t>
   </si>
   <si>
-    <t>Dead wood C concentration (%) [decay class 3]</t>
-  </si>
-  <si>
-    <t>Harmon et al. (2013)</t>
-  </si>
-  <si>
-    <t>Dead material CV</t>
-  </si>
-  <si>
-    <t>Dead material standard deviation</t>
-  </si>
-  <si>
     <t>Dead wood accumulation rate (t C/ha/y)</t>
   </si>
   <si>
     <t>Total ecosystem (30 cm)</t>
-  </si>
-  <si>
-    <t>Total ecosystem (12 cm)</t>
-  </si>
-  <si>
-    <t>Aboveground woody biomass &lt;20 y (t/ha)</t>
-  </si>
-  <si>
-    <t>Mean age of younger sites</t>
-  </si>
-  <si>
-    <t>Mean age of older sites</t>
   </si>
   <si>
     <t>Aboveground biomass</t>
@@ -726,7 +677,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1">
         <v>1998</v>
@@ -747,18 +698,18 @@
         <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>2023</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D2">
         <v>0.69</v>
@@ -775,19 +726,19 @@
         <v>0.12</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <f>B2-B1</f>
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>0.92</v>
@@ -820,7 +771,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>0.82</v>
@@ -839,12 +790,12 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <f>C26/$D$10</f>
@@ -859,23 +810,23 @@
         <v>0.62</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>34.700000000000003</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D9">
         <v>0.47799999999999998</v>
@@ -887,23 +838,23 @@
         <v>0.52</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3">
         <f>C28/$D$10</f>
@@ -920,7 +871,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -932,12 +883,12 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -951,7 +902,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14">
         <v>0.48</v>
@@ -963,12 +914,12 @@
         <v>0.5</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D15">
         <v>130</v>
@@ -980,12 +931,12 @@
         <v>200</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D16">
         <v>60</v>
@@ -999,7 +950,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D17">
         <v>0.46</v>
@@ -1011,12 +962,12 @@
         <v>0.93</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <v>0.23</v>
@@ -1030,7 +981,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D19">
         <v>0.24</v>
@@ -1050,16 +1001,16 @@
         <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1084,7 +1035,7 @@
     </row>
     <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C23" s="6">
         <f>C24*D5</f>
@@ -1113,15 +1064,15 @@
         <v>88</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="6">
         <f>D7*$B$3</f>
@@ -1138,7 +1089,7 @@
     </row>
     <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="6">
         <v>13</v>
@@ -1150,15 +1101,15 @@
         <v>31</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="6">
         <f>D11*$B$3</f>
@@ -1175,7 +1126,7 @@
     </row>
     <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="6">
         <f>$D$8*D9</f>
@@ -1192,10 +1143,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="2">
         <f>C25+C27</f>
@@ -1212,7 +1163,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2">
         <f>C26+C28</f>
@@ -1229,10 +1180,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="2">
         <f>D12*20+D13*5</f>
@@ -1249,7 +1200,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32">
         <f>D15</f>
@@ -1266,10 +1217,10 @@
     </row>
     <row r="33" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33" s="6">
         <f>C31*D14</f>
@@ -1286,7 +1237,7 @@
     </row>
     <row r="34" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="6">
         <f>C32*D14</f>
@@ -1303,10 +1254,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" s="3">
         <f>IF(C31&lt;75, $D$17, IF(C31&gt;150, $D$19, $D$18))</f>
@@ -1323,7 +1274,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="3">
         <f>IF(C32&lt;75, $D$17, IF(C32&gt;150, $D$19, $D$18))</f>
@@ -1340,10 +1291,10 @@
     </row>
     <row r="37" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37" s="6">
         <f t="shared" ref="C37:E38" si="4">C33*C35</f>
@@ -1360,7 +1311,7 @@
     </row>
     <row r="38" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38" s="6">
         <f t="shared" si="4"/>
@@ -1377,10 +1328,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C39" s="2">
         <f>C33+C37</f>
@@ -1397,7 +1348,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C40" s="2">
         <f>C34+C38</f>
@@ -1414,10 +1365,10 @@
     </row>
     <row r="41" spans="1:5" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C41" s="6">
         <f t="shared" ref="C41:E42" si="7">C23+C25+C27+C33+C37</f>
@@ -1434,7 +1385,7 @@
     </row>
     <row r="42" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" si="7"/>
@@ -1469,45 +1420,45 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="J2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1702,7 +1653,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C9">
         <f>SUM(C3:C8)</f>
@@ -1723,7 +1674,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <f>C9+H9</f>
@@ -1736,7 +1687,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D11" s="4">
         <f>D10/C10/100</f>
@@ -1745,7 +1696,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D12">
         <f>MIN(E3:E8,J4:J7)/100</f>
@@ -1754,590 +1705,11 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D13">
         <f>MAX(F3:F8,K4:K7)/100</f>
         <v>0.52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B88190-6FA7-43C6-8927-D04E5F92F0A3}">
-  <dimension ref="A1:H33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1">
-        <v>1998</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>2022</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2">
-        <v>0.69</v>
-      </c>
-      <c r="E2">
-        <f>D2-G2</f>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="F2">
-        <f>D2+G2</f>
-        <v>0.80999999999999994</v>
-      </c>
-      <c r="G2">
-        <v>0.12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3">
-        <f>(14+19)/2</f>
-        <v>16.5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3">
-        <v>0.92</v>
-      </c>
-      <c r="E3">
-        <f>D3-G3</f>
-        <v>0.78</v>
-      </c>
-      <c r="F3">
-        <f>D3+G3</f>
-        <v>1.06</v>
-      </c>
-      <c r="G3">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4">
-        <f>(24+29)/2</f>
-        <v>26.5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5">
-        <v>0.82</v>
-      </c>
-      <c r="E5">
-        <f>D5-G5</f>
-        <v>0.64999999999999991</v>
-      </c>
-      <c r="F5">
-        <f>D5+G5</f>
-        <v>0.99</v>
-      </c>
-      <c r="G5">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7">
-        <f>C25/$D$12</f>
-        <v>0.26</v>
-      </c>
-      <c r="E7">
-        <f>D25/$D$12</f>
-        <v>0.04</v>
-      </c>
-      <c r="F7">
-        <f>E25/$D$12</f>
-        <v>0.62</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10">
-        <f>D8*D9</f>
-        <v>34.700000000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="E11">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="F11">
-        <v>0.51300000000000001</v>
-      </c>
-      <c r="H11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12">
-        <v>50</v>
-      </c>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="3">
-        <f>C27/$D$12</f>
-        <v>0.333814</v>
-      </c>
-      <c r="E13" s="3">
-        <f>D27/$D$12</f>
-        <v>0.31577000000000005</v>
-      </c>
-      <c r="F13" s="3">
-        <f>E27/$D$12</f>
-        <v>0.35602200000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>0.5</v>
-      </c>
-      <c r="F14">
-        <v>8</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>0.5</v>
-      </c>
-      <c r="F15">
-        <v>7.5</v>
-      </c>
-      <c r="H15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16">
-        <v>0.48</v>
-      </c>
-      <c r="E16">
-        <v>0.46</v>
-      </c>
-      <c r="F16">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17">
-        <v>130</v>
-      </c>
-      <c r="E17">
-        <v>50</v>
-      </c>
-      <c r="F17">
-        <v>200</v>
-      </c>
-      <c r="H17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18">
-        <v>60</v>
-      </c>
-      <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="F18">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="2">
-        <f>C23*D2*D3*D4</f>
-        <v>55.862400000000001</v>
-      </c>
-      <c r="D21" s="2">
-        <f>D23*E2*E3*E4</f>
-        <v>39.1248</v>
-      </c>
-      <c r="E21" s="2">
-        <f>E23*F2*F3*F4</f>
-        <v>75.55680000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="2">
-        <f>C23*D5</f>
-        <v>72.16</v>
-      </c>
-      <c r="D22" s="2">
-        <f>D23*E5</f>
-        <v>57.199999999999989</v>
-      </c>
-      <c r="E22" s="2">
-        <f>E23*F5</f>
-        <v>87.12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2">
-        <v>88</v>
-      </c>
-      <c r="D23" s="2">
-        <v>88</v>
-      </c>
-      <c r="E23" s="2">
-        <v>88</v>
-      </c>
-      <c r="F23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="2">
-        <f>D7*$B$3</f>
-        <v>4.29</v>
-      </c>
-      <c r="D24" s="2">
-        <f>E7*$B$3</f>
-        <v>0.66</v>
-      </c>
-      <c r="E24" s="2">
-        <f>F7*$B$3</f>
-        <v>10.23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="2">
-        <v>13</v>
-      </c>
-      <c r="D25" s="2">
-        <v>2</v>
-      </c>
-      <c r="E25" s="2">
-        <v>31</v>
-      </c>
-      <c r="F25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="2">
-        <f>D13*$B$3</f>
-        <v>5.5079310000000001</v>
-      </c>
-      <c r="D26" s="2">
-        <f>E13*$B$3</f>
-        <v>5.2102050000000011</v>
-      </c>
-      <c r="E26" s="2">
-        <f>F13*$B$3</f>
-        <v>5.8743630000000007</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="2">
-        <f>$D$8*D11</f>
-        <v>16.6907</v>
-      </c>
-      <c r="D27" s="2">
-        <f>$D$8*E11</f>
-        <v>15.788500000000003</v>
-      </c>
-      <c r="E27" s="2">
-        <f>$D$8*F11</f>
-        <v>17.801100000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="2">
-        <f>D16*(D14*20+D15*4)</f>
-        <v>46.08</v>
-      </c>
-      <c r="D28" s="2">
-        <f>E16*(E14*20+E15*4)</f>
-        <v>5.5200000000000005</v>
-      </c>
-      <c r="E28" s="2">
-        <f>F16*(F14*20+F15*4)</f>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="2">
-        <f>D16*D17</f>
-        <v>62.4</v>
-      </c>
-      <c r="D29" s="2">
-        <f>E16*E17</f>
-        <v>23</v>
-      </c>
-      <c r="E29" s="2">
-        <f>F16*F17</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="2">
-        <f>$C$22+$C$24+$C$26+$C$28</f>
-        <v>128.03793100000001</v>
-      </c>
-      <c r="D30" s="2">
-        <f>$D$22+$D$24+$D$26+$D$28</f>
-        <v>68.590204999999983</v>
-      </c>
-      <c r="E30" s="2">
-        <f>$E$22+$E$24+$E$26+$E$28</f>
-        <v>198.22436300000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="2">
-        <f>$C$23+$C$25+$C$27+$C$29</f>
-        <v>180.0907</v>
-      </c>
-      <c r="D31" s="2">
-        <f>$D$23+$D$25+$D$27+$D$29</f>
-        <v>128.7885</v>
-      </c>
-      <c r="E31" s="2">
-        <f>$E$23+$E$25+$E$27+$E$29</f>
-        <v>236.80109999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="2">
-        <f>$C$22*(12/30)+$C$24+$C$26+$C$28</f>
-        <v>84.741930999999994</v>
-      </c>
-      <c r="D32" s="2">
-        <f>$D$22*(12/30)+$D$24+$D$26+$D$28</f>
-        <v>34.270204999999997</v>
-      </c>
-      <c r="E32" s="2">
-        <f>$E$22*(12/30)+$E$24+$E$26+$E$28</f>
-        <v>145.95236299999999</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="2">
-        <f>$C$23*(12/30)+$C$25+$C$27+$C$29</f>
-        <v>127.29070000000002</v>
-      </c>
-      <c r="D33" s="2">
-        <f>$D$23*(12/30)+$D$25+$D$27+$D$29</f>
-        <v>75.988500000000002</v>
-      </c>
-      <c r="E33" s="2">
-        <f>$E$23*(12/30)+$E$25+$E$27+$E$29</f>
-        <v>184.00110000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>